<commit_message>
Move research time application to ATLS vs standard care trial directory
</commit_message>
<xml_diff>
--- a/agreements/Frågor från juristen för att granska avtal SVE.xlsx
+++ b/agreements/Frågor från juristen för att granska avtal SVE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kise-my.sharepoint.com/personal/therese_lind_ki_se/Documents/Skrivbordet/Avtal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/Documents/trauma-life-support-training-effectiveness-research-network/atls-vs-standard-care-trial/agreements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{75461EF3-3C15-4064-8259-88D23C028CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E8BC36D-7325-45C7-848F-823122659293}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750A6F1B-FFDD-3049-8AFF-70793870119C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4018572D-D321-43B4-87C3-FB2D90C15FAD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{4018572D-D321-43B4-87C3-FB2D90C15FAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <r>
       <rPr>
@@ -472,6 +472,42 @@
       </rPr>
       <t>Annat</t>
     </r>
+  </si>
+  <si>
+    <t>Administrativ chef</t>
+  </si>
+  <si>
+    <t>Martin Gerdin Wärnberg</t>
+  </si>
+  <si>
+    <t>Nej</t>
+  </si>
+  <si>
+    <t>ca 5 miljoner SEK</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Vetenskapsrådet</t>
+  </si>
+  <si>
+    <t>Ej tillämpligt</t>
+  </si>
+  <si>
+    <t>The George Institute (TGI, India), University of Birmingham (UoB, UK)</t>
+  </si>
+  <si>
+    <t>Ja. Det behövs ett RCA mellan KI, TGI och UoB samt ett JCA mellan KI och TGI</t>
+  </si>
+  <si>
+    <t>Nej, inte än. KI är ensam huvudman.</t>
+  </si>
+  <si>
+    <t>Ja. Bidraget är "bidrag för forskningstid i klinisk miljö".</t>
+  </si>
+  <si>
+    <t>Ja. Pseudonymiserade hälsodata. Samlas in av TGI och överförs till KI för lagring och analys.</t>
   </si>
 </sst>
 </file>
@@ -661,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -700,8 +736,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -731,7 +766,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1019,7 +1054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1030,565 +1065,591 @@
   <dimension ref="A1:BM31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="155.28515625" customWidth="1"/>
+    <col min="1" max="1" width="155.33203125" customWidth="1"/>
     <col min="2" max="2" width="85" customWidth="1"/>
-    <col min="3" max="65" width="9.140625" style="20"/>
+    <col min="3" max="65" width="9.1640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:65" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="5"/>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:65" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="7"/>
-    </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:65" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:65" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:65" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="20"/>
-      <c r="U9" s="20"/>
-      <c r="V9" s="20"/>
-      <c r="W9" s="20"/>
-      <c r="X9" s="20"/>
-      <c r="Y9" s="20"/>
-      <c r="Z9" s="20"/>
-      <c r="AA9" s="20"/>
-      <c r="AB9" s="20"/>
-      <c r="AC9" s="20"/>
-      <c r="AD9" s="20"/>
-      <c r="AE9" s="20"/>
-      <c r="AF9" s="20"/>
-      <c r="AG9" s="20"/>
-      <c r="AH9" s="20"/>
-      <c r="AI9" s="20"/>
-      <c r="AJ9" s="20"/>
-      <c r="AK9" s="20"/>
-      <c r="AL9" s="20"/>
-      <c r="AM9" s="20"/>
-      <c r="AN9" s="20"/>
-      <c r="AO9" s="20"/>
-      <c r="AP9" s="20"/>
-      <c r="AQ9" s="20"/>
-      <c r="AR9" s="20"/>
-      <c r="AS9" s="20"/>
-      <c r="AT9" s="20"/>
-      <c r="AU9" s="20"/>
-      <c r="AV9" s="20"/>
-      <c r="AW9" s="20"/>
-      <c r="AX9" s="20"/>
-      <c r="AY9" s="20"/>
-      <c r="AZ9" s="20"/>
-      <c r="BA9" s="20"/>
-      <c r="BB9" s="20"/>
-      <c r="BC9" s="20"/>
-      <c r="BD9" s="20"/>
-      <c r="BE9" s="20"/>
-      <c r="BF9" s="20"/>
-      <c r="BG9" s="20"/>
-      <c r="BH9" s="20"/>
-      <c r="BI9" s="20"/>
-      <c r="BJ9" s="20"/>
-      <c r="BK9" s="20"/>
-      <c r="BL9" s="20"/>
-      <c r="BM9" s="20"/>
-    </row>
-    <row r="10" spans="1:65" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+      <c r="Z9"/>
+      <c r="AA9"/>
+      <c r="AB9"/>
+      <c r="AC9"/>
+      <c r="AD9"/>
+      <c r="AE9"/>
+      <c r="AF9"/>
+      <c r="AG9"/>
+      <c r="AH9"/>
+      <c r="AI9"/>
+      <c r="AJ9"/>
+      <c r="AK9"/>
+      <c r="AL9"/>
+      <c r="AM9"/>
+      <c r="AN9"/>
+      <c r="AO9"/>
+      <c r="AP9"/>
+      <c r="AQ9"/>
+      <c r="AR9"/>
+      <c r="AS9"/>
+      <c r="AT9"/>
+      <c r="AU9"/>
+      <c r="AV9"/>
+      <c r="AW9"/>
+      <c r="AX9"/>
+      <c r="AY9"/>
+      <c r="AZ9"/>
+      <c r="BA9"/>
+      <c r="BB9"/>
+      <c r="BC9"/>
+      <c r="BD9"/>
+      <c r="BE9"/>
+      <c r="BF9"/>
+      <c r="BG9"/>
+      <c r="BH9"/>
+      <c r="BI9"/>
+      <c r="BJ9"/>
+      <c r="BK9"/>
+      <c r="BL9"/>
+      <c r="BM9"/>
+    </row>
+    <row r="10" spans="1:65" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20"/>
-      <c r="U10" s="20"/>
-      <c r="V10" s="20"/>
-      <c r="W10" s="20"/>
-      <c r="X10" s="20"/>
-      <c r="Y10" s="20"/>
-      <c r="Z10" s="20"/>
-      <c r="AA10" s="20"/>
-      <c r="AB10" s="20"/>
-      <c r="AC10" s="20"/>
-      <c r="AD10" s="20"/>
-      <c r="AE10" s="20"/>
-      <c r="AF10" s="20"/>
-      <c r="AG10" s="20"/>
-      <c r="AH10" s="20"/>
-      <c r="AI10" s="20"/>
-      <c r="AJ10" s="20"/>
-      <c r="AK10" s="20"/>
-      <c r="AL10" s="20"/>
-      <c r="AM10" s="20"/>
-      <c r="AN10" s="20"/>
-      <c r="AO10" s="20"/>
-      <c r="AP10" s="20"/>
-      <c r="AQ10" s="20"/>
-      <c r="AR10" s="20"/>
-      <c r="AS10" s="20"/>
-      <c r="AT10" s="20"/>
-      <c r="AU10" s="20"/>
-      <c r="AV10" s="20"/>
-      <c r="AW10" s="20"/>
-      <c r="AX10" s="20"/>
-      <c r="AY10" s="20"/>
-      <c r="AZ10" s="20"/>
-      <c r="BA10" s="20"/>
-      <c r="BB10" s="20"/>
-      <c r="BC10" s="20"/>
-      <c r="BD10" s="20"/>
-      <c r="BE10" s="20"/>
-      <c r="BF10" s="20"/>
-      <c r="BG10" s="20"/>
-      <c r="BH10" s="20"/>
-      <c r="BI10" s="20"/>
-      <c r="BJ10" s="20"/>
-      <c r="BK10" s="20"/>
-      <c r="BL10" s="20"/>
-      <c r="BM10" s="20"/>
-    </row>
-    <row r="11" spans="1:65" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+      <c r="AA10"/>
+      <c r="AB10"/>
+      <c r="AC10"/>
+      <c r="AD10"/>
+      <c r="AE10"/>
+      <c r="AF10"/>
+      <c r="AG10"/>
+      <c r="AH10"/>
+      <c r="AI10"/>
+      <c r="AJ10"/>
+      <c r="AK10"/>
+      <c r="AL10"/>
+      <c r="AM10"/>
+      <c r="AN10"/>
+      <c r="AO10"/>
+      <c r="AP10"/>
+      <c r="AQ10"/>
+      <c r="AR10"/>
+      <c r="AS10"/>
+      <c r="AT10"/>
+      <c r="AU10"/>
+      <c r="AV10"/>
+      <c r="AW10"/>
+      <c r="AX10"/>
+      <c r="AY10"/>
+      <c r="AZ10"/>
+      <c r="BA10"/>
+      <c r="BB10"/>
+      <c r="BC10"/>
+      <c r="BD10"/>
+      <c r="BE10"/>
+      <c r="BF10"/>
+      <c r="BG10"/>
+      <c r="BH10"/>
+      <c r="BI10"/>
+      <c r="BJ10"/>
+      <c r="BK10"/>
+      <c r="BL10"/>
+      <c r="BM10"/>
+    </row>
+    <row r="11" spans="1:65" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="20"/>
-      <c r="U11" s="20"/>
-      <c r="V11" s="20"/>
-      <c r="W11" s="20"/>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="20"/>
-      <c r="Z11" s="20"/>
-      <c r="AA11" s="20"/>
-      <c r="AB11" s="20"/>
-      <c r="AC11" s="20"/>
-      <c r="AD11" s="20"/>
-      <c r="AE11" s="20"/>
-      <c r="AF11" s="20"/>
-      <c r="AG11" s="20"/>
-      <c r="AH11" s="20"/>
-      <c r="AI11" s="20"/>
-      <c r="AJ11" s="20"/>
-      <c r="AK11" s="20"/>
-      <c r="AL11" s="20"/>
-      <c r="AM11" s="20"/>
-      <c r="AN11" s="20"/>
-      <c r="AO11" s="20"/>
-      <c r="AP11" s="20"/>
-      <c r="AQ11" s="20"/>
-      <c r="AR11" s="20"/>
-      <c r="AS11" s="20"/>
-      <c r="AT11" s="20"/>
-      <c r="AU11" s="20"/>
-      <c r="AV11" s="20"/>
-      <c r="AW11" s="20"/>
-      <c r="AX11" s="20"/>
-      <c r="AY11" s="20"/>
-      <c r="AZ11" s="20"/>
-      <c r="BA11" s="20"/>
-      <c r="BB11" s="20"/>
-      <c r="BC11" s="20"/>
-      <c r="BD11" s="20"/>
-      <c r="BE11" s="20"/>
-      <c r="BF11" s="20"/>
-      <c r="BG11" s="20"/>
-      <c r="BH11" s="20"/>
-      <c r="BI11" s="20"/>
-      <c r="BJ11" s="20"/>
-      <c r="BK11" s="20"/>
-      <c r="BL11" s="20"/>
-      <c r="BM11" s="20"/>
-    </row>
-    <row r="12" spans="1:65" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="Y11"/>
+      <c r="Z11"/>
+      <c r="AA11"/>
+      <c r="AB11"/>
+      <c r="AC11"/>
+      <c r="AD11"/>
+      <c r="AE11"/>
+      <c r="AF11"/>
+      <c r="AG11"/>
+      <c r="AH11"/>
+      <c r="AI11"/>
+      <c r="AJ11"/>
+      <c r="AK11"/>
+      <c r="AL11"/>
+      <c r="AM11"/>
+      <c r="AN11"/>
+      <c r="AO11"/>
+      <c r="AP11"/>
+      <c r="AQ11"/>
+      <c r="AR11"/>
+      <c r="AS11"/>
+      <c r="AT11"/>
+      <c r="AU11"/>
+      <c r="AV11"/>
+      <c r="AW11"/>
+      <c r="AX11"/>
+      <c r="AY11"/>
+      <c r="AZ11"/>
+      <c r="BA11"/>
+      <c r="BB11"/>
+      <c r="BC11"/>
+      <c r="BD11"/>
+      <c r="BE11"/>
+      <c r="BF11"/>
+      <c r="BG11"/>
+      <c r="BH11"/>
+      <c r="BI11"/>
+      <c r="BJ11"/>
+      <c r="BK11"/>
+      <c r="BL11"/>
+      <c r="BM11"/>
+    </row>
+    <row r="12" spans="1:65" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="20"/>
-      <c r="U12" s="20"/>
-      <c r="V12" s="20"/>
-      <c r="W12" s="20"/>
-      <c r="X12" s="20"/>
-      <c r="Y12" s="20"/>
-      <c r="Z12" s="20"/>
-      <c r="AA12" s="20"/>
-      <c r="AB12" s="20"/>
-      <c r="AC12" s="20"/>
-      <c r="AD12" s="20"/>
-      <c r="AE12" s="20"/>
-      <c r="AF12" s="20"/>
-      <c r="AG12" s="20"/>
-      <c r="AH12" s="20"/>
-      <c r="AI12" s="20"/>
-      <c r="AJ12" s="20"/>
-      <c r="AK12" s="20"/>
-      <c r="AL12" s="20"/>
-      <c r="AM12" s="20"/>
-      <c r="AN12" s="20"/>
-      <c r="AO12" s="20"/>
-      <c r="AP12" s="20"/>
-      <c r="AQ12" s="20"/>
-      <c r="AR12" s="20"/>
-      <c r="AS12" s="20"/>
-      <c r="AT12" s="20"/>
-      <c r="AU12" s="20"/>
-      <c r="AV12" s="20"/>
-      <c r="AW12" s="20"/>
-      <c r="AX12" s="20"/>
-      <c r="AY12" s="20"/>
-      <c r="AZ12" s="20"/>
-      <c r="BA12" s="20"/>
-      <c r="BB12" s="20"/>
-      <c r="BC12" s="20"/>
-      <c r="BD12" s="20"/>
-      <c r="BE12" s="20"/>
-      <c r="BF12" s="20"/>
-      <c r="BG12" s="20"/>
-      <c r="BH12" s="20"/>
-      <c r="BI12" s="20"/>
-      <c r="BJ12" s="20"/>
-      <c r="BK12" s="20"/>
-      <c r="BL12" s="20"/>
-      <c r="BM12" s="20"/>
-    </row>
-    <row r="13" spans="1:65" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="B12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+      <c r="Z12"/>
+      <c r="AA12"/>
+      <c r="AB12"/>
+      <c r="AC12"/>
+      <c r="AD12"/>
+      <c r="AE12"/>
+      <c r="AF12"/>
+      <c r="AG12"/>
+      <c r="AH12"/>
+      <c r="AI12"/>
+      <c r="AJ12"/>
+      <c r="AK12"/>
+      <c r="AL12"/>
+      <c r="AM12"/>
+      <c r="AN12"/>
+      <c r="AO12"/>
+      <c r="AP12"/>
+      <c r="AQ12"/>
+      <c r="AR12"/>
+      <c r="AS12"/>
+      <c r="AT12"/>
+      <c r="AU12"/>
+      <c r="AV12"/>
+      <c r="AW12"/>
+      <c r="AX12"/>
+      <c r="AY12"/>
+      <c r="AZ12"/>
+      <c r="BA12"/>
+      <c r="BB12"/>
+      <c r="BC12"/>
+      <c r="BD12"/>
+      <c r="BE12"/>
+      <c r="BF12"/>
+      <c r="BG12"/>
+      <c r="BH12"/>
+      <c r="BI12"/>
+      <c r="BJ12"/>
+      <c r="BK12"/>
+      <c r="BL12"/>
+      <c r="BM12"/>
+    </row>
+    <row r="13" spans="1:65" s="18" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="20"/>
-      <c r="T13" s="20"/>
-      <c r="U13" s="20"/>
-      <c r="V13" s="20"/>
-      <c r="W13" s="20"/>
-      <c r="X13" s="20"/>
-      <c r="Y13" s="20"/>
-      <c r="Z13" s="20"/>
-      <c r="AA13" s="20"/>
-      <c r="AB13" s="20"/>
-      <c r="AC13" s="20"/>
-      <c r="AD13" s="20"/>
-      <c r="AE13" s="20"/>
-      <c r="AF13" s="20"/>
-      <c r="AG13" s="20"/>
-      <c r="AH13" s="20"/>
-      <c r="AI13" s="20"/>
-      <c r="AJ13" s="20"/>
-      <c r="AK13" s="20"/>
-      <c r="AL13" s="20"/>
-      <c r="AM13" s="20"/>
-      <c r="AN13" s="20"/>
-      <c r="AO13" s="20"/>
-      <c r="AP13" s="20"/>
-      <c r="AQ13" s="20"/>
-      <c r="AR13" s="20"/>
-      <c r="AS13" s="20"/>
-      <c r="AT13" s="20"/>
-      <c r="AU13" s="20"/>
-      <c r="AV13" s="20"/>
-      <c r="AW13" s="20"/>
-      <c r="AX13" s="20"/>
-      <c r="AY13" s="20"/>
-      <c r="AZ13" s="20"/>
-      <c r="BA13" s="20"/>
-      <c r="BB13" s="20"/>
-      <c r="BC13" s="20"/>
-      <c r="BD13" s="20"/>
-      <c r="BE13" s="20"/>
-      <c r="BF13" s="20"/>
-      <c r="BG13" s="20"/>
-      <c r="BH13" s="20"/>
-      <c r="BI13" s="20"/>
-      <c r="BJ13" s="20"/>
-      <c r="BK13" s="20"/>
-      <c r="BL13" s="20"/>
-      <c r="BM13" s="20"/>
-    </row>
-    <row r="14" spans="1:65" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
+      <c r="Z13"/>
+      <c r="AA13"/>
+      <c r="AB13"/>
+      <c r="AC13"/>
+      <c r="AD13"/>
+      <c r="AE13"/>
+      <c r="AF13"/>
+      <c r="AG13"/>
+      <c r="AH13"/>
+      <c r="AI13"/>
+      <c r="AJ13"/>
+      <c r="AK13"/>
+      <c r="AL13"/>
+      <c r="AM13"/>
+      <c r="AN13"/>
+      <c r="AO13"/>
+      <c r="AP13"/>
+      <c r="AQ13"/>
+      <c r="AR13"/>
+      <c r="AS13"/>
+      <c r="AT13"/>
+      <c r="AU13"/>
+      <c r="AV13"/>
+      <c r="AW13"/>
+      <c r="AX13"/>
+      <c r="AY13"/>
+      <c r="AZ13"/>
+      <c r="BA13"/>
+      <c r="BB13"/>
+      <c r="BC13"/>
+      <c r="BD13"/>
+      <c r="BE13"/>
+      <c r="BF13"/>
+      <c r="BG13"/>
+      <c r="BH13"/>
+      <c r="BI13"/>
+      <c r="BJ13"/>
+      <c r="BK13"/>
+      <c r="BL13"/>
+      <c r="BM13"/>
+    </row>
+    <row r="14" spans="1:65" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="20"/>
-      <c r="U14" s="20"/>
-      <c r="V14" s="20"/>
-      <c r="W14" s="20"/>
-      <c r="X14" s="20"/>
-      <c r="Y14" s="20"/>
-      <c r="Z14" s="20"/>
-      <c r="AA14" s="20"/>
-      <c r="AB14" s="20"/>
-      <c r="AC14" s="20"/>
-      <c r="AD14" s="20"/>
-      <c r="AE14" s="20"/>
-      <c r="AF14" s="20"/>
-      <c r="AG14" s="20"/>
-      <c r="AH14" s="20"/>
-      <c r="AI14" s="20"/>
-      <c r="AJ14" s="20"/>
-      <c r="AK14" s="20"/>
-      <c r="AL14" s="20"/>
-      <c r="AM14" s="20"/>
-      <c r="AN14" s="20"/>
-      <c r="AO14" s="20"/>
-      <c r="AP14" s="20"/>
-      <c r="AQ14" s="20"/>
-      <c r="AR14" s="20"/>
-      <c r="AS14" s="20"/>
-      <c r="AT14" s="20"/>
-      <c r="AU14" s="20"/>
-      <c r="AV14" s="20"/>
-      <c r="AW14" s="20"/>
-      <c r="AX14" s="20"/>
-      <c r="AY14" s="20"/>
-      <c r="AZ14" s="20"/>
-      <c r="BA14" s="20"/>
-      <c r="BB14" s="20"/>
-      <c r="BC14" s="20"/>
-      <c r="BD14" s="20"/>
-      <c r="BE14" s="20"/>
-      <c r="BF14" s="20"/>
-      <c r="BG14" s="20"/>
-      <c r="BH14" s="20"/>
-      <c r="BI14" s="20"/>
-      <c r="BJ14" s="20"/>
-      <c r="BK14" s="20"/>
-      <c r="BL14" s="20"/>
-      <c r="BM14" s="20"/>
-    </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="B14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+      <c r="AB14"/>
+      <c r="AC14"/>
+      <c r="AD14"/>
+      <c r="AE14"/>
+      <c r="AF14"/>
+      <c r="AG14"/>
+      <c r="AH14"/>
+      <c r="AI14"/>
+      <c r="AJ14"/>
+      <c r="AK14"/>
+      <c r="AL14"/>
+      <c r="AM14"/>
+      <c r="AN14"/>
+      <c r="AO14"/>
+      <c r="AP14"/>
+      <c r="AQ14"/>
+      <c r="AR14"/>
+      <c r="AS14"/>
+      <c r="AT14"/>
+      <c r="AU14"/>
+      <c r="AV14"/>
+      <c r="AW14"/>
+      <c r="AX14"/>
+      <c r="AY14"/>
+      <c r="AZ14"/>
+      <c r="BA14"/>
+      <c r="BB14"/>
+      <c r="BC14"/>
+      <c r="BD14"/>
+      <c r="BE14"/>
+      <c r="BF14"/>
+      <c r="BG14"/>
+      <c r="BH14"/>
+      <c r="BI14"/>
+      <c r="BJ14"/>
+      <c r="BK14"/>
+      <c r="BL14"/>
+      <c r="BM14"/>
+    </row>
+    <row r="15" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="7"/>
-    </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="B16" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="11"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="11"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="21"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="20"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="11"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="11"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="11"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="11"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B26" s="11"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="11"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="11"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="9"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
     </row>
   </sheetData>

</xml_diff>